<commit_message>
Update Bugdet and Role play - add role table to master sheet
</commit_message>
<xml_diff>
--- a/InteractivePowellBudget/InteractiveLakePowellWaterBudgetAndRolePlay.xlsx
+++ b/InteractivePowellBudget/InteractiveLakePowellWaterBudgetAndRolePlay.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Research\ColoradoRiver\RCode\ColoradoRiverFutures\InteractivePowellBudget\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3215398A-B1A6-4D5E-8E0A-12CEBECE85A1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C409FB75-6FB0-42FD-925C-F6DCDBA12C3E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6640" xr2:uid="{5373AB19-D84C-490D-97DC-C516D358024A}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6640" activeTab="1" xr2:uid="{5373AB19-D84C-490D-97DC-C516D358024A}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe-Directions" sheetId="6" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="141">
   <si>
     <t>Mexico obligation</t>
   </si>
@@ -205,9 +205,6 @@
     <t>Strategy</t>
   </si>
   <si>
-    <t>??</t>
-  </si>
-  <si>
     <t>Release 0.75 maf per year allocation each year</t>
   </si>
   <si>
@@ -218,9 +215,6 @@
   </si>
   <si>
     <t>Interactive Water Budget and Accounting for Lake Powell Watershed</t>
-  </si>
-  <si>
-    <t>Consume 4.5 maf per year or try to increase</t>
   </si>
   <si>
     <t>Explanation of Cell Types</t>
@@ -475,7 +469,7 @@
     <numFmt numFmtId="166" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="167" formatCode="&quot;$&quot;#,##0"/>
     <numFmt numFmtId="168" formatCode="0."/>
-    <numFmt numFmtId="171" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="169" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -706,7 +700,7 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -749,9 +743,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -773,6 +764,24 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="5" fillId="5" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -780,16 +789,6 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -810,17 +809,8 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="5" fillId="5" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -9943,7 +9933,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{447CC9A2-4C52-453A-A3CD-EA6E59E26162}">
   <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView topLeftCell="A11" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="A27" sqref="A27:L27"/>
     </sheetView>
   </sheetViews>
@@ -9963,7 +9953,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="2"/>
@@ -9984,20 +9974,20 @@
       <c r="D3"/>
     </row>
     <row r="4" spans="1:12" ht="134" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="20" t="s">
-        <v>74</v>
-      </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
-      <c r="K4" s="20"/>
-      <c r="L4" s="20"/>
+      <c r="A4" s="44" t="s">
+        <v>72</v>
+      </c>
+      <c r="B4" s="44"/>
+      <c r="C4" s="44"/>
+      <c r="D4" s="44"/>
+      <c r="E4" s="44"/>
+      <c r="F4" s="44"/>
+      <c r="G4" s="44"/>
+      <c r="H4" s="44"/>
+      <c r="I4" s="44"/>
+      <c r="J4" s="44"/>
+      <c r="K4" s="44"/>
+      <c r="L4" s="44"/>
     </row>
     <row r="5" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="16"/>
@@ -10013,310 +10003,315 @@
       <c r="L5" s="16"/>
     </row>
     <row r="6" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="30" t="s">
-        <v>69</v>
-      </c>
-      <c r="B6" s="31"/>
-      <c r="C6" s="31"/>
-      <c r="D6" s="31"/>
-      <c r="E6" s="31"/>
-      <c r="F6" s="31"/>
-      <c r="G6" s="31"/>
-      <c r="H6" s="31"/>
-      <c r="I6" s="31"/>
-      <c r="J6" s="31"/>
-      <c r="K6" s="31"/>
-      <c r="L6" s="32"/>
+      <c r="A6" s="35" t="s">
+        <v>67</v>
+      </c>
+      <c r="B6" s="36"/>
+      <c r="C6" s="36"/>
+      <c r="D6" s="36"/>
+      <c r="E6" s="36"/>
+      <c r="F6" s="36"/>
+      <c r="G6" s="36"/>
+      <c r="H6" s="36"/>
+      <c r="I6" s="36"/>
+      <c r="J6" s="36"/>
+      <c r="K6" s="36"/>
+      <c r="L6" s="37"/>
     </row>
     <row r="7" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="43">
+      <c r="A7" s="30">
         <v>1</v>
       </c>
-      <c r="B7" s="37" t="s">
-        <v>138</v>
-      </c>
-      <c r="C7" s="37"/>
-      <c r="D7" s="37"/>
-      <c r="E7" s="37"/>
-      <c r="F7" s="37"/>
-      <c r="G7" s="37"/>
-      <c r="H7" s="37"/>
-      <c r="I7" s="37"/>
-      <c r="J7" s="37"/>
-      <c r="K7" s="37"/>
-      <c r="L7" s="38"/>
+      <c r="B7" s="38" t="s">
+        <v>136</v>
+      </c>
+      <c r="C7" s="38"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="38"/>
+      <c r="F7" s="38"/>
+      <c r="G7" s="38"/>
+      <c r="H7" s="38"/>
+      <c r="I7" s="38"/>
+      <c r="J7" s="38"/>
+      <c r="K7" s="38"/>
+      <c r="L7" s="39"/>
     </row>
     <row r="8" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="43">
+      <c r="A8" s="30">
         <v>2</v>
       </c>
-      <c r="B8" s="37" t="s">
+      <c r="B8" s="38" t="s">
+        <v>118</v>
+      </c>
+      <c r="C8" s="38"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="38"/>
+      <c r="G8" s="38"/>
+      <c r="H8" s="38"/>
+      <c r="I8" s="38"/>
+      <c r="J8" s="38"/>
+      <c r="K8" s="38"/>
+      <c r="L8" s="39"/>
+    </row>
+    <row r="9" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="30">
+        <v>3</v>
+      </c>
+      <c r="B9" s="38" t="s">
+        <v>73</v>
+      </c>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="38"/>
+      <c r="H9" s="38"/>
+      <c r="I9" s="38"/>
+      <c r="J9" s="38"/>
+      <c r="K9" s="38"/>
+      <c r="L9" s="39"/>
+    </row>
+    <row r="10" spans="1:12" ht="32.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="30">
+        <v>4</v>
+      </c>
+      <c r="B10" s="38" t="s">
+        <v>119</v>
+      </c>
+      <c r="C10" s="38"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="38"/>
+      <c r="I10" s="38"/>
+      <c r="J10" s="38"/>
+      <c r="K10" s="38"/>
+      <c r="L10" s="39"/>
+    </row>
+    <row r="11" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="30">
+        <v>5</v>
+      </c>
+      <c r="B11" s="38" t="s">
+        <v>75</v>
+      </c>
+      <c r="C11" s="38"/>
+      <c r="D11" s="38"/>
+      <c r="E11" s="38"/>
+      <c r="F11" s="38"/>
+      <c r="G11" s="38"/>
+      <c r="H11" s="38"/>
+      <c r="I11" s="38"/>
+      <c r="J11" s="38"/>
+      <c r="K11" s="38"/>
+      <c r="L11" s="39"/>
+    </row>
+    <row r="12" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="30">
+        <v>6</v>
+      </c>
+      <c r="B12" s="38" t="s">
+        <v>76</v>
+      </c>
+      <c r="C12" s="38"/>
+      <c r="D12" s="38"/>
+      <c r="E12" s="38"/>
+      <c r="F12" s="38"/>
+      <c r="G12" s="38"/>
+      <c r="H12" s="38"/>
+      <c r="I12" s="38"/>
+      <c r="J12" s="38"/>
+      <c r="K12" s="38"/>
+      <c r="L12" s="39"/>
+    </row>
+    <row r="13" spans="1:12" ht="32.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="30">
+        <v>7</v>
+      </c>
+      <c r="B13" s="38" t="s">
         <v>120</v>
       </c>
-      <c r="C8" s="37"/>
-      <c r="D8" s="37"/>
-      <c r="E8" s="37"/>
-      <c r="F8" s="37"/>
-      <c r="G8" s="37"/>
-      <c r="H8" s="37"/>
-      <c r="I8" s="37"/>
-      <c r="J8" s="37"/>
-      <c r="K8" s="37"/>
-      <c r="L8" s="38"/>
-    </row>
-    <row r="9" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="43">
-        <v>3</v>
-      </c>
-      <c r="B9" s="37" t="s">
-        <v>75</v>
-      </c>
-      <c r="C9" s="37"/>
-      <c r="D9" s="37"/>
-      <c r="E9" s="37"/>
-      <c r="F9" s="37"/>
-      <c r="G9" s="37"/>
-      <c r="H9" s="37"/>
-      <c r="I9" s="37"/>
-      <c r="J9" s="37"/>
-      <c r="K9" s="37"/>
-      <c r="L9" s="38"/>
-    </row>
-    <row r="10" spans="1:12" ht="32.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="43">
-        <v>4</v>
-      </c>
-      <c r="B10" s="37" t="s">
+      <c r="C13" s="38"/>
+      <c r="D13" s="38"/>
+      <c r="E13" s="38"/>
+      <c r="F13" s="38"/>
+      <c r="G13" s="38"/>
+      <c r="H13" s="38"/>
+      <c r="I13" s="38"/>
+      <c r="J13" s="38"/>
+      <c r="K13" s="38"/>
+      <c r="L13" s="39"/>
+    </row>
+    <row r="14" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="30">
+        <v>8</v>
+      </c>
+      <c r="B14" s="38" t="s">
+        <v>77</v>
+      </c>
+      <c r="C14" s="38"/>
+      <c r="D14" s="38"/>
+      <c r="E14" s="38"/>
+      <c r="F14" s="38"/>
+      <c r="G14" s="38"/>
+      <c r="H14" s="38"/>
+      <c r="I14" s="38"/>
+      <c r="J14" s="38"/>
+      <c r="K14" s="38"/>
+      <c r="L14" s="39"/>
+    </row>
+    <row r="15" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="30">
+        <v>9</v>
+      </c>
+      <c r="B15" s="38" t="s">
         <v>121</v>
       </c>
-      <c r="C10" s="37"/>
-      <c r="D10" s="37"/>
-      <c r="E10" s="37"/>
-      <c r="F10" s="37"/>
-      <c r="G10" s="37"/>
-      <c r="H10" s="37"/>
-      <c r="I10" s="37"/>
-      <c r="J10" s="37"/>
-      <c r="K10" s="37"/>
-      <c r="L10" s="38"/>
-    </row>
-    <row r="11" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="43">
-        <v>5</v>
-      </c>
-      <c r="B11" s="37" t="s">
-        <v>77</v>
-      </c>
-      <c r="C11" s="37"/>
-      <c r="D11" s="37"/>
-      <c r="E11" s="37"/>
-      <c r="F11" s="37"/>
-      <c r="G11" s="37"/>
-      <c r="H11" s="37"/>
-      <c r="I11" s="37"/>
-      <c r="J11" s="37"/>
-      <c r="K11" s="37"/>
-      <c r="L11" s="38"/>
-    </row>
-    <row r="12" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="43">
-        <v>6</v>
-      </c>
-      <c r="B12" s="37" t="s">
+      <c r="C15" s="38"/>
+      <c r="D15" s="38"/>
+      <c r="E15" s="38"/>
+      <c r="F15" s="38"/>
+      <c r="G15" s="38"/>
+      <c r="H15" s="38"/>
+      <c r="I15" s="38"/>
+      <c r="J15" s="38"/>
+      <c r="K15" s="38"/>
+      <c r="L15" s="39"/>
+    </row>
+    <row r="16" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="30">
+        <v>10</v>
+      </c>
+      <c r="B16" s="38" t="s">
         <v>78</v>
       </c>
-      <c r="C12" s="37"/>
-      <c r="D12" s="37"/>
-      <c r="E12" s="37"/>
-      <c r="F12" s="37"/>
-      <c r="G12" s="37"/>
-      <c r="H12" s="37"/>
-      <c r="I12" s="37"/>
-      <c r="J12" s="37"/>
-      <c r="K12" s="37"/>
-      <c r="L12" s="38"/>
-    </row>
-    <row r="13" spans="1:12" ht="32.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="43">
-        <v>7</v>
-      </c>
-      <c r="B13" s="37" t="s">
-        <v>122</v>
-      </c>
-      <c r="C13" s="37"/>
-      <c r="D13" s="37"/>
-      <c r="E13" s="37"/>
-      <c r="F13" s="37"/>
-      <c r="G13" s="37"/>
-      <c r="H13" s="37"/>
-      <c r="I13" s="37"/>
-      <c r="J13" s="37"/>
-      <c r="K13" s="37"/>
-      <c r="L13" s="38"/>
-    </row>
-    <row r="14" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="43">
-        <v>8</v>
-      </c>
-      <c r="B14" s="37" t="s">
+      <c r="C16" s="38"/>
+      <c r="D16" s="38"/>
+      <c r="E16" s="38"/>
+      <c r="F16" s="38"/>
+      <c r="G16" s="38"/>
+      <c r="H16" s="38"/>
+      <c r="I16" s="38"/>
+      <c r="J16" s="38"/>
+      <c r="K16" s="38"/>
+      <c r="L16" s="39"/>
+    </row>
+    <row r="17" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="30">
+        <v>11</v>
+      </c>
+      <c r="B17" s="40" t="s">
         <v>79</v>
       </c>
-      <c r="C14" s="37"/>
-      <c r="D14" s="37"/>
-      <c r="E14" s="37"/>
-      <c r="F14" s="37"/>
-      <c r="G14" s="37"/>
-      <c r="H14" s="37"/>
-      <c r="I14" s="37"/>
-      <c r="J14" s="37"/>
-      <c r="K14" s="37"/>
-      <c r="L14" s="38"/>
-    </row>
-    <row r="15" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="43">
-        <v>9</v>
-      </c>
-      <c r="B15" s="37" t="s">
-        <v>123</v>
-      </c>
-      <c r="C15" s="37"/>
-      <c r="D15" s="37"/>
-      <c r="E15" s="37"/>
-      <c r="F15" s="37"/>
-      <c r="G15" s="37"/>
-      <c r="H15" s="37"/>
-      <c r="I15" s="37"/>
-      <c r="J15" s="37"/>
-      <c r="K15" s="37"/>
-      <c r="L15" s="38"/>
-    </row>
-    <row r="16" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="43">
-        <v>10</v>
-      </c>
-      <c r="B16" s="37" t="s">
-        <v>80</v>
-      </c>
-      <c r="C16" s="37"/>
-      <c r="D16" s="37"/>
-      <c r="E16" s="37"/>
-      <c r="F16" s="37"/>
-      <c r="G16" s="37"/>
-      <c r="H16" s="37"/>
-      <c r="I16" s="37"/>
-      <c r="J16" s="37"/>
-      <c r="K16" s="37"/>
-      <c r="L16" s="38"/>
-    </row>
-    <row r="17" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="43">
-        <v>11</v>
-      </c>
-      <c r="B17" s="39" t="s">
-        <v>81</v>
-      </c>
-      <c r="C17" s="39"/>
-      <c r="D17" s="39"/>
-      <c r="E17" s="39"/>
-      <c r="F17" s="39"/>
-      <c r="G17" s="39"/>
-      <c r="H17" s="39"/>
-      <c r="I17" s="39"/>
-      <c r="J17" s="39"/>
-      <c r="K17" s="39"/>
-      <c r="L17" s="40"/>
+      <c r="C17" s="40"/>
+      <c r="D17" s="40"/>
+      <c r="E17" s="40"/>
+      <c r="F17" s="40"/>
+      <c r="G17" s="40"/>
+      <c r="H17" s="40"/>
+      <c r="I17" s="40"/>
+      <c r="J17" s="40"/>
+      <c r="K17" s="40"/>
+      <c r="L17" s="41"/>
     </row>
     <row r="18" spans="1:12" ht="32" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="43">
+      <c r="A18" s="30">
         <v>12</v>
       </c>
-      <c r="B18" s="41" t="s">
-        <v>139</v>
-      </c>
-      <c r="C18" s="41"/>
-      <c r="D18" s="41"/>
-      <c r="E18" s="41"/>
-      <c r="F18" s="41"/>
-      <c r="G18" s="41"/>
-      <c r="H18" s="41"/>
-      <c r="I18" s="41"/>
-      <c r="J18" s="41"/>
-      <c r="K18" s="41"/>
-      <c r="L18" s="42"/>
+      <c r="B18" s="42" t="s">
+        <v>137</v>
+      </c>
+      <c r="C18" s="42"/>
+      <c r="D18" s="42"/>
+      <c r="E18" s="42"/>
+      <c r="F18" s="42"/>
+      <c r="G18" s="42"/>
+      <c r="H18" s="42"/>
+      <c r="I18" s="42"/>
+      <c r="J18" s="42"/>
+      <c r="K18" s="42"/>
+      <c r="L18" s="43"/>
     </row>
     <row r="19" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="29"/>
-      <c r="C19" s="29"/>
-      <c r="D19" s="29"/>
-      <c r="E19" s="29"/>
-      <c r="F19" s="29"/>
-      <c r="G19" s="29"/>
-      <c r="H19" s="29"/>
-      <c r="I19" s="29"/>
-      <c r="J19" s="29"/>
-      <c r="K19" s="29"/>
-      <c r="L19" s="29"/>
+      <c r="B19" s="28"/>
+      <c r="C19" s="28"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="28"/>
+      <c r="F19" s="28"/>
+      <c r="G19" s="28"/>
+      <c r="H19" s="28"/>
+      <c r="I19" s="28"/>
+      <c r="J19" s="28"/>
+      <c r="K19" s="28"/>
+      <c r="L19" s="28"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B21" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C21" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B22" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C22" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B23" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C23" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B24" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C24" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="27" spans="1:12" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="36" t="s">
-        <v>140</v>
-      </c>
-      <c r="B27" s="36"/>
-      <c r="C27" s="36"/>
-      <c r="D27" s="36"/>
-      <c r="E27" s="36"/>
-      <c r="F27" s="36"/>
-      <c r="G27" s="36"/>
-      <c r="H27" s="36"/>
-      <c r="I27" s="36"/>
-      <c r="J27" s="36"/>
-      <c r="K27" s="36"/>
-      <c r="L27" s="36"/>
+      <c r="A27" s="34" t="s">
+        <v>138</v>
+      </c>
+      <c r="B27" s="34"/>
+      <c r="C27" s="34"/>
+      <c r="D27" s="34"/>
+      <c r="E27" s="34"/>
+      <c r="F27" s="34"/>
+      <c r="G27" s="34"/>
+      <c r="H27" s="34"/>
+      <c r="I27" s="34"/>
+      <c r="J27" s="34"/>
+      <c r="K27" s="34"/>
+      <c r="L27" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A4:L4"/>
+    <mergeCell ref="B9:L9"/>
+    <mergeCell ref="B11:L11"/>
+    <mergeCell ref="B12:L12"/>
+    <mergeCell ref="B13:L13"/>
     <mergeCell ref="A27:L27"/>
     <mergeCell ref="A6:L6"/>
     <mergeCell ref="B10:L10"/>
@@ -10327,11 +10322,6 @@
     <mergeCell ref="B16:L16"/>
     <mergeCell ref="B17:L17"/>
     <mergeCell ref="B18:L18"/>
-    <mergeCell ref="A4:L4"/>
-    <mergeCell ref="B9:L9"/>
-    <mergeCell ref="B11:L11"/>
-    <mergeCell ref="B12:L12"/>
-    <mergeCell ref="B13:L13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -10341,8 +10331,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3356767-5983-45FB-80E4-1C5DE08E38A0}">
   <dimension ref="A1:L52"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -10360,7 +10350,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B1" s="1"/>
     </row>
@@ -10369,19 +10359,19 @@
       <c r="B2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="29" t="s">
-        <v>71</v>
-      </c>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29"/>
-      <c r="J3" s="29"/>
-      <c r="K3" s="29"/>
+      <c r="A3" s="28" t="s">
+        <v>69</v>
+      </c>
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="28"/>
+      <c r="I3" s="28"/>
+      <c r="J3" s="28"/>
+      <c r="K3" s="28"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="18" t="s">
@@ -10395,38 +10385,52 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A5" s="33" t="s">
-        <v>72</v>
-      </c>
-      <c r="B5" s="34"/>
-      <c r="C5" s="35"/>
+      <c r="A5" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="B5" s="13"/>
+      <c r="C5" s="45"/>
+      <c r="D5" s="46"/>
+      <c r="E5" s="46"/>
+      <c r="F5" s="46"/>
+      <c r="G5" s="46"/>
+      <c r="H5" s="46"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" t="s">
-        <v>62</v>
-      </c>
+      <c r="B6" s="13"/>
+      <c r="C6" s="45"/>
+      <c r="D6" s="46"/>
+      <c r="E6" s="46"/>
+      <c r="F6" s="46"/>
+      <c r="G6" s="46"/>
+      <c r="H6" s="46"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="B7" s="2"/>
-      <c r="C7" t="s">
-        <v>57</v>
-      </c>
+      <c r="B7" s="13"/>
+      <c r="C7" s="45"/>
+      <c r="D7" s="46"/>
+      <c r="E7" s="46"/>
+      <c r="F7" s="46"/>
+      <c r="G7" s="46"/>
+      <c r="H7" s="46"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="B8" s="2"/>
-      <c r="C8" t="s">
-        <v>58</v>
-      </c>
+      <c r="B8" s="13"/>
+      <c r="C8" s="45"/>
+      <c r="D8" s="46"/>
+      <c r="E8" s="46"/>
+      <c r="F8" s="46"/>
+      <c r="G8" s="46"/>
+      <c r="H8" s="46"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="17"/>
@@ -10434,33 +10438,33 @@
       <c r="C9"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A10" s="21" t="s">
-        <v>63</v>
+      <c r="A10" s="20" t="s">
+        <v>61</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A11" s="22" t="s">
-        <v>73</v>
+      <c r="A11" s="21" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A12" s="24" t="s">
-        <v>65</v>
-      </c>
-      <c r="B12" s="21"/>
+      <c r="A12" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="B12" s="20"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A13" s="23" t="s">
-        <v>64</v>
+      <c r="A13" s="22" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="D15" s="22"/>
+        <v>74</v>
+      </c>
+      <c r="D15" s="21"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
@@ -10475,8 +10479,8 @@
       <c r="B18" s="12">
         <v>5.73</v>
       </c>
-      <c r="C18" s="25" t="s">
-        <v>68</v>
+      <c r="C18" s="24" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.35">
@@ -10495,7 +10499,7 @@
         <v>47</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C21" s="14" t="s">
         <v>9</v>
@@ -10530,7 +10534,7 @@
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="12"/>
@@ -10594,7 +10598,7 @@
       <c r="A24" t="s">
         <v>35</v>
       </c>
-      <c r="B24" s="26">
+      <c r="B24" s="25">
         <v>1</v>
       </c>
       <c r="C24" s="15" t="str">
@@ -10642,7 +10646,7 @@
       <c r="A25" t="s">
         <v>36</v>
       </c>
-      <c r="B25" s="26">
+      <c r="B25" s="25">
         <v>0</v>
       </c>
       <c r="C25" s="15" t="str">
@@ -10690,7 +10694,7 @@
       <c r="A26" t="s">
         <v>37</v>
       </c>
-      <c r="B26" s="26">
+      <c r="B26" s="25">
         <v>0</v>
       </c>
       <c r="C26" s="15" t="str">
@@ -10736,7 +10740,7 @@
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B27" s="1"/>
       <c r="C27" s="15" t="str">
@@ -10785,42 +10789,42 @@
         <v>0</v>
       </c>
       <c r="B28" s="1"/>
-      <c r="C28" s="27">
+      <c r="C28" s="26">
         <v>0.75</v>
       </c>
-      <c r="D28" s="27">
+      <c r="D28" s="26">
         <f>C28</f>
         <v>0.75</v>
       </c>
-      <c r="E28" s="27">
+      <c r="E28" s="26">
         <f t="shared" ref="E28:L28" si="3">D28</f>
         <v>0.75</v>
       </c>
-      <c r="F28" s="27">
+      <c r="F28" s="26">
         <f t="shared" si="3"/>
         <v>0.75</v>
       </c>
-      <c r="G28" s="27">
+      <c r="G28" s="26">
         <f t="shared" si="3"/>
         <v>0.75</v>
       </c>
-      <c r="H28" s="27">
+      <c r="H28" s="26">
         <f t="shared" si="3"/>
         <v>0.75</v>
       </c>
-      <c r="I28" s="27">
+      <c r="I28" s="26">
         <f t="shared" si="3"/>
         <v>0.75</v>
       </c>
-      <c r="J28" s="27">
+      <c r="J28" s="26">
         <f t="shared" si="3"/>
         <v>0.75</v>
       </c>
-      <c r="K28" s="27">
+      <c r="K28" s="26">
         <f t="shared" si="3"/>
         <v>0.75</v>
       </c>
-      <c r="L28" s="27">
+      <c r="L28" s="26">
         <f t="shared" si="3"/>
         <v>0.75</v>
       </c>
@@ -10875,7 +10879,7 @@
       <c r="A30" t="s">
         <v>1</v>
       </c>
-      <c r="B30" s="26">
+      <c r="B30" s="25">
         <v>0.5</v>
       </c>
       <c r="C30" s="15" t="str">
@@ -10923,7 +10927,7 @@
       <c r="A31" t="s">
         <v>2</v>
       </c>
-      <c r="B31" s="26">
+      <c r="B31" s="25">
         <f>1-B30</f>
         <v>0.5</v>
       </c>
@@ -10973,32 +10977,32 @@
         <v>41</v>
       </c>
       <c r="B32" s="1"/>
-      <c r="C32" s="27"/>
-      <c r="D32" s="27"/>
-      <c r="E32" s="27"/>
-      <c r="F32" s="27"/>
-      <c r="G32" s="27"/>
-      <c r="H32" s="27"/>
-      <c r="I32" s="27"/>
-      <c r="J32" s="27"/>
-      <c r="K32" s="27"/>
-      <c r="L32" s="27"/>
+      <c r="C32" s="26"/>
+      <c r="D32" s="26"/>
+      <c r="E32" s="26"/>
+      <c r="F32" s="26"/>
+      <c r="G32" s="26"/>
+      <c r="H32" s="26"/>
+      <c r="I32" s="26"/>
+      <c r="J32" s="26"/>
+      <c r="K32" s="26"/>
+      <c r="L32" s="26"/>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>42</v>
       </c>
       <c r="B33" s="1"/>
-      <c r="C33" s="27"/>
-      <c r="D33" s="27"/>
-      <c r="E33" s="27"/>
-      <c r="F33" s="27"/>
-      <c r="G33" s="27"/>
-      <c r="H33" s="27"/>
-      <c r="I33" s="27"/>
-      <c r="J33" s="27"/>
-      <c r="K33" s="27"/>
-      <c r="L33" s="27"/>
+      <c r="C33" s="26"/>
+      <c r="D33" s="26"/>
+      <c r="E33" s="26"/>
+      <c r="F33" s="26"/>
+      <c r="G33" s="26"/>
+      <c r="H33" s="26"/>
+      <c r="I33" s="26"/>
+      <c r="J33" s="26"/>
+      <c r="K33" s="26"/>
+      <c r="L33" s="26"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
@@ -11101,50 +11105,50 @@
       <c r="A37" t="s">
         <v>7</v>
       </c>
-      <c r="C37" s="28" t="str">
+      <c r="C37" s="27" t="str">
         <f>IF(C$22&lt;&gt;"",C26+C28,"")</f>
         <v/>
       </c>
-      <c r="D37" s="28" t="str">
+      <c r="D37" s="27" t="str">
         <f>IF(D$22&lt;&gt;"",D26+D28,"")</f>
         <v/>
       </c>
-      <c r="E37" s="28" t="str">
+      <c r="E37" s="27" t="str">
         <f t="shared" ref="E37:L37" si="8">IF(E$22&lt;&gt;"",E26+E28,"")</f>
         <v/>
       </c>
-      <c r="F37" s="28" t="str">
+      <c r="F37" s="27" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
-      <c r="G37" s="28" t="str">
+      <c r="G37" s="27" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
-      <c r="H37" s="28" t="str">
+      <c r="H37" s="27" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
-      <c r="I37" s="28" t="str">
+      <c r="I37" s="27" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
-      <c r="J37" s="28" t="str">
+      <c r="J37" s="27" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
-      <c r="K37" s="28" t="str">
+      <c r="K37" s="27" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
-      <c r="L37" s="28" t="str">
+      <c r="L37" s="27" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B38" s="1"/>
       <c r="D38" s="2"/>
@@ -11161,46 +11165,46 @@
       <c r="A39" t="s">
         <v>5</v>
       </c>
-      <c r="C39" s="27"/>
-      <c r="D39" s="27"/>
-      <c r="E39" s="27"/>
-      <c r="F39" s="27"/>
-      <c r="G39" s="27"/>
-      <c r="H39" s="27"/>
-      <c r="I39" s="27"/>
-      <c r="J39" s="27"/>
-      <c r="K39" s="27"/>
-      <c r="L39" s="27"/>
+      <c r="C39" s="26"/>
+      <c r="D39" s="26"/>
+      <c r="E39" s="26"/>
+      <c r="F39" s="26"/>
+      <c r="G39" s="26"/>
+      <c r="H39" s="26"/>
+      <c r="I39" s="26"/>
+      <c r="J39" s="26"/>
+      <c r="K39" s="26"/>
+      <c r="L39" s="26"/>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>6</v>
       </c>
-      <c r="C40" s="27"/>
-      <c r="D40" s="27"/>
-      <c r="E40" s="27"/>
-      <c r="F40" s="27"/>
-      <c r="G40" s="27"/>
-      <c r="H40" s="27"/>
-      <c r="I40" s="27"/>
-      <c r="J40" s="27"/>
-      <c r="K40" s="27"/>
-      <c r="L40" s="27"/>
+      <c r="C40" s="26"/>
+      <c r="D40" s="26"/>
+      <c r="E40" s="26"/>
+      <c r="F40" s="26"/>
+      <c r="G40" s="26"/>
+      <c r="H40" s="26"/>
+      <c r="I40" s="26"/>
+      <c r="J40" s="26"/>
+      <c r="K40" s="26"/>
+      <c r="L40" s="26"/>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>7</v>
       </c>
-      <c r="C41" s="27"/>
-      <c r="D41" s="27"/>
-      <c r="E41" s="27"/>
-      <c r="F41" s="27"/>
-      <c r="G41" s="27"/>
-      <c r="H41" s="27"/>
-      <c r="I41" s="27"/>
-      <c r="J41" s="27"/>
-      <c r="K41" s="27"/>
-      <c r="L41" s="27"/>
+      <c r="C41" s="26"/>
+      <c r="D41" s="26"/>
+      <c r="E41" s="26"/>
+      <c r="F41" s="26"/>
+      <c r="G41" s="26"/>
+      <c r="H41" s="26"/>
+      <c r="I41" s="26"/>
+      <c r="J41" s="26"/>
+      <c r="K41" s="26"/>
+      <c r="L41" s="26"/>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
@@ -11448,6 +11452,12 @@
       <c r="D52" s="19"/>
     </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="C5:H5"/>
+    <mergeCell ref="C6:H6"/>
+    <mergeCell ref="C7:H7"/>
+    <mergeCell ref="C8:H8"/>
+  </mergeCells>
   <conditionalFormatting sqref="C39:L39">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
       <formula>$C$35</formula>
@@ -11462,7 +11472,7 @@
   <dimension ref="A1:L52"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="B5" sqref="B5:H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -11480,7 +11490,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B1" s="1"/>
     </row>
@@ -11489,19 +11499,19 @@
       <c r="B2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="29" t="s">
-        <v>71</v>
-      </c>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29"/>
-      <c r="J3" s="29"/>
-      <c r="K3" s="29"/>
+      <c r="A3" s="28" t="s">
+        <v>69</v>
+      </c>
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="28"/>
+      <c r="I3" s="28"/>
+      <c r="J3" s="28"/>
+      <c r="K3" s="28"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="18" t="s">
@@ -11515,68 +11525,68 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A5" s="33" t="s">
-        <v>72</v>
+      <c r="A5" s="29" t="s">
+        <v>70</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>133</v>
-      </c>
-      <c r="C5" s="47" t="s">
-        <v>136</v>
-      </c>
-      <c r="D5" s="48"/>
-      <c r="E5" s="48"/>
-      <c r="F5" s="48"/>
-      <c r="G5" s="48"/>
-      <c r="H5" s="48"/>
+        <v>131</v>
+      </c>
+      <c r="C5" s="45" t="s">
+        <v>134</v>
+      </c>
+      <c r="D5" s="46"/>
+      <c r="E5" s="46"/>
+      <c r="F5" s="46"/>
+      <c r="G5" s="46"/>
+      <c r="H5" s="46"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="17" t="s">
         <v>52</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>133</v>
-      </c>
-      <c r="C6" s="47" t="s">
-        <v>134</v>
-      </c>
-      <c r="D6" s="48"/>
-      <c r="E6" s="48"/>
-      <c r="F6" s="48"/>
-      <c r="G6" s="48"/>
-      <c r="H6" s="48"/>
+        <v>131</v>
+      </c>
+      <c r="C6" s="45" t="s">
+        <v>132</v>
+      </c>
+      <c r="D6" s="46"/>
+      <c r="E6" s="46"/>
+      <c r="F6" s="46"/>
+      <c r="G6" s="46"/>
+      <c r="H6" s="46"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="17" t="s">
         <v>53</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>133</v>
-      </c>
-      <c r="C7" s="47" t="s">
-        <v>137</v>
-      </c>
-      <c r="D7" s="48"/>
-      <c r="E7" s="48"/>
-      <c r="F7" s="48"/>
-      <c r="G7" s="48"/>
-      <c r="H7" s="48"/>
+        <v>131</v>
+      </c>
+      <c r="C7" s="45" t="s">
+        <v>135</v>
+      </c>
+      <c r="D7" s="46"/>
+      <c r="E7" s="46"/>
+      <c r="F7" s="46"/>
+      <c r="G7" s="46"/>
+      <c r="H7" s="46"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="17" t="s">
         <v>54</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>133</v>
-      </c>
-      <c r="C8" s="47" t="s">
-        <v>58</v>
-      </c>
-      <c r="D8" s="48"/>
-      <c r="E8" s="48"/>
-      <c r="F8" s="48"/>
-      <c r="G8" s="48"/>
-      <c r="H8" s="48"/>
+        <v>131</v>
+      </c>
+      <c r="C8" s="45" t="s">
+        <v>57</v>
+      </c>
+      <c r="D8" s="46"/>
+      <c r="E8" s="46"/>
+      <c r="F8" s="46"/>
+      <c r="G8" s="46"/>
+      <c r="H8" s="46"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="17"/>
@@ -11584,39 +11594,39 @@
       <c r="C9"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A10" s="21" t="s">
-        <v>63</v>
+      <c r="A10" s="20" t="s">
+        <v>61</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A11" s="22" t="s">
-        <v>73</v>
+      <c r="A11" s="21" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A12" s="24" t="s">
-        <v>65</v>
-      </c>
-      <c r="B12" s="21"/>
+      <c r="A12" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="B12" s="20"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A13" s="23" t="s">
-        <v>64</v>
+      <c r="A13" s="22" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="D15" s="49" t="s">
-        <v>135</v>
-      </c>
-      <c r="E15" s="50"/>
-      <c r="F15" s="50"/>
-      <c r="G15" s="50"/>
-      <c r="H15" s="51"/>
+        <v>74</v>
+      </c>
+      <c r="D15" s="47" t="s">
+        <v>133</v>
+      </c>
+      <c r="E15" s="48"/>
+      <c r="F15" s="48"/>
+      <c r="G15" s="48"/>
+      <c r="H15" s="49"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
@@ -11631,8 +11641,8 @@
       <c r="B18" s="12">
         <v>5.73</v>
       </c>
-      <c r="C18" s="25" t="s">
-        <v>68</v>
+      <c r="C18" s="24" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.35">
@@ -11651,7 +11661,7 @@
         <v>47</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C21" s="14" t="s">
         <v>9</v>
@@ -11686,7 +11696,7 @@
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="12">
@@ -11770,7 +11780,7 @@
       <c r="A24" t="s">
         <v>35</v>
       </c>
-      <c r="B24" s="26">
+      <c r="B24" s="25">
         <v>1</v>
       </c>
       <c r="C24" s="15">
@@ -11818,7 +11828,7 @@
       <c r="A25" t="s">
         <v>36</v>
       </c>
-      <c r="B25" s="26">
+      <c r="B25" s="25">
         <v>0</v>
       </c>
       <c r="C25" s="15">
@@ -11866,7 +11876,7 @@
       <c r="A26" t="s">
         <v>37</v>
       </c>
-      <c r="B26" s="26">
+      <c r="B26" s="25">
         <v>0</v>
       </c>
       <c r="C26" s="15">
@@ -11912,7 +11922,7 @@
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B27" s="1"/>
       <c r="C27" s="15">
@@ -11961,42 +11971,42 @@
         <v>0</v>
       </c>
       <c r="B28" s="1"/>
-      <c r="C28" s="27">
+      <c r="C28" s="26">
         <v>0.75</v>
       </c>
-      <c r="D28" s="27">
+      <c r="D28" s="26">
         <f>C28</f>
         <v>0.75</v>
       </c>
-      <c r="E28" s="27">
+      <c r="E28" s="26">
         <f t="shared" ref="E28:L28" si="3">D28</f>
         <v>0.75</v>
       </c>
-      <c r="F28" s="27">
+      <c r="F28" s="26">
         <f t="shared" si="3"/>
         <v>0.75</v>
       </c>
-      <c r="G28" s="27">
+      <c r="G28" s="26">
         <f t="shared" si="3"/>
         <v>0.75</v>
       </c>
-      <c r="H28" s="27">
+      <c r="H28" s="26">
         <f t="shared" si="3"/>
         <v>0.75</v>
       </c>
-      <c r="I28" s="27">
+      <c r="I28" s="26">
         <f t="shared" si="3"/>
         <v>0.75</v>
       </c>
-      <c r="J28" s="27">
+      <c r="J28" s="26">
         <f t="shared" si="3"/>
         <v>0.75</v>
       </c>
-      <c r="K28" s="27">
+      <c r="K28" s="26">
         <f t="shared" si="3"/>
         <v>0.75</v>
       </c>
-      <c r="L28" s="27">
+      <c r="L28" s="26">
         <f t="shared" si="3"/>
         <v>0.75</v>
       </c>
@@ -12051,7 +12061,7 @@
       <c r="A30" t="s">
         <v>1</v>
       </c>
-      <c r="B30" s="26">
+      <c r="B30" s="25">
         <v>0.5</v>
       </c>
       <c r="C30" s="15">
@@ -12099,7 +12109,7 @@
       <c r="A31" t="s">
         <v>2</v>
       </c>
-      <c r="B31" s="26">
+      <c r="B31" s="25">
         <f>1-B30</f>
         <v>0.5</v>
       </c>
@@ -12149,42 +12159,42 @@
         <v>41</v>
       </c>
       <c r="B32" s="1"/>
-      <c r="C32" s="27">
+      <c r="C32" s="26">
         <v>1.3</v>
       </c>
-      <c r="D32" s="27">
+      <c r="D32" s="26">
         <f>C32</f>
         <v>1.3</v>
       </c>
-      <c r="E32" s="27">
+      <c r="E32" s="26">
         <f t="shared" ref="E32:L32" si="6">D32</f>
         <v>1.3</v>
       </c>
-      <c r="F32" s="27">
+      <c r="F32" s="26">
         <f t="shared" si="6"/>
         <v>1.3</v>
       </c>
-      <c r="G32" s="27">
+      <c r="G32" s="26">
         <f t="shared" si="6"/>
         <v>1.3</v>
       </c>
-      <c r="H32" s="27">
+      <c r="H32" s="26">
         <f t="shared" si="6"/>
         <v>1.3</v>
       </c>
-      <c r="I32" s="27">
+      <c r="I32" s="26">
         <f t="shared" si="6"/>
         <v>1.3</v>
       </c>
-      <c r="J32" s="27">
+      <c r="J32" s="26">
         <f t="shared" si="6"/>
         <v>1.3</v>
       </c>
-      <c r="K32" s="27">
+      <c r="K32" s="26">
         <f t="shared" si="6"/>
         <v>1.3</v>
       </c>
-      <c r="L32" s="27">
+      <c r="L32" s="26">
         <f t="shared" si="6"/>
         <v>1.3</v>
       </c>
@@ -12194,19 +12204,19 @@
         <v>42</v>
       </c>
       <c r="B33" s="1"/>
-      <c r="C33" s="46">
+      <c r="C33" s="33">
         <f>C32*300</f>
         <v>390</v>
       </c>
-      <c r="D33" s="27"/>
-      <c r="E33" s="27"/>
-      <c r="F33" s="27"/>
-      <c r="G33" s="27"/>
-      <c r="H33" s="27"/>
-      <c r="I33" s="27"/>
-      <c r="J33" s="27"/>
-      <c r="K33" s="27"/>
-      <c r="L33" s="27"/>
+      <c r="D33" s="26"/>
+      <c r="E33" s="26"/>
+      <c r="F33" s="26"/>
+      <c r="G33" s="26"/>
+      <c r="H33" s="26"/>
+      <c r="I33" s="26"/>
+      <c r="J33" s="26"/>
+      <c r="K33" s="26"/>
+      <c r="L33" s="26"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
@@ -12309,50 +12319,50 @@
       <c r="A37" t="s">
         <v>7</v>
       </c>
-      <c r="C37" s="28">
+      <c r="C37" s="27">
         <f>IF(C$22&lt;&gt;"",C26+C28,"")</f>
         <v>0.75</v>
       </c>
-      <c r="D37" s="28">
+      <c r="D37" s="27">
         <f>IF(D$22&lt;&gt;"",D26+D28,"")</f>
         <v>0.75</v>
       </c>
-      <c r="E37" s="28">
+      <c r="E37" s="27">
         <f t="shared" ref="E37:L37" si="9">IF(E$22&lt;&gt;"",E26+E28,"")</f>
         <v>0.75</v>
       </c>
-      <c r="F37" s="28">
+      <c r="F37" s="27">
         <f t="shared" si="9"/>
         <v>0.75</v>
       </c>
-      <c r="G37" s="28">
+      <c r="G37" s="27">
         <f t="shared" si="9"/>
         <v>0.75</v>
       </c>
-      <c r="H37" s="28">
+      <c r="H37" s="27">
         <f t="shared" si="9"/>
         <v>0.75</v>
       </c>
-      <c r="I37" s="28">
+      <c r="I37" s="27">
         <f t="shared" si="9"/>
         <v>0.75</v>
       </c>
-      <c r="J37" s="28">
+      <c r="J37" s="27">
         <f t="shared" si="9"/>
         <v>0.75</v>
       </c>
-      <c r="K37" s="28">
+      <c r="K37" s="27">
         <f t="shared" si="9"/>
         <v>0.75</v>
       </c>
-      <c r="L37" s="28">
+      <c r="L37" s="27">
         <f t="shared" si="9"/>
         <v>0.75</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B38" s="1"/>
       <c r="D38" s="2"/>
@@ -12369,42 +12379,42 @@
       <c r="A39" t="s">
         <v>5</v>
       </c>
-      <c r="C39" s="27">
+      <c r="C39" s="26">
         <v>4.5</v>
       </c>
-      <c r="D39" s="27">
+      <c r="D39" s="26">
         <f>C39</f>
         <v>4.5</v>
       </c>
-      <c r="E39" s="27">
+      <c r="E39" s="26">
         <f t="shared" ref="E39:L39" si="10">D39</f>
         <v>4.5</v>
       </c>
-      <c r="F39" s="27">
+      <c r="F39" s="26">
         <f t="shared" si="10"/>
         <v>4.5</v>
       </c>
-      <c r="G39" s="27">
+      <c r="G39" s="26">
         <f t="shared" si="10"/>
         <v>4.5</v>
       </c>
-      <c r="H39" s="27">
+      <c r="H39" s="26">
         <f t="shared" si="10"/>
         <v>4.5</v>
       </c>
-      <c r="I39" s="27">
+      <c r="I39" s="26">
         <f t="shared" si="10"/>
         <v>4.5</v>
       </c>
-      <c r="J39" s="27">
+      <c r="J39" s="26">
         <f t="shared" si="10"/>
         <v>4.5</v>
       </c>
-      <c r="K39" s="27">
+      <c r="K39" s="26">
         <f t="shared" si="10"/>
         <v>4.5</v>
       </c>
-      <c r="L39" s="27">
+      <c r="L39" s="26">
         <f t="shared" si="10"/>
         <v>4.5</v>
       </c>
@@ -12413,42 +12423,42 @@
       <c r="A40" t="s">
         <v>6</v>
       </c>
-      <c r="C40" s="27">
+      <c r="C40" s="26">
         <v>6.6</v>
       </c>
-      <c r="D40" s="27">
+      <c r="D40" s="26">
         <f t="shared" ref="D40:L41" si="11">C40</f>
         <v>6.6</v>
       </c>
-      <c r="E40" s="27">
+      <c r="E40" s="26">
         <f t="shared" si="11"/>
         <v>6.6</v>
       </c>
-      <c r="F40" s="27">
+      <c r="F40" s="26">
         <f t="shared" si="11"/>
         <v>6.6</v>
       </c>
-      <c r="G40" s="27">
+      <c r="G40" s="26">
         <f t="shared" si="11"/>
         <v>6.6</v>
       </c>
-      <c r="H40" s="27">
+      <c r="H40" s="26">
         <f t="shared" si="11"/>
         <v>6.6</v>
       </c>
-      <c r="I40" s="27">
+      <c r="I40" s="26">
         <f t="shared" si="11"/>
         <v>6.6</v>
       </c>
-      <c r="J40" s="27">
+      <c r="J40" s="26">
         <f t="shared" si="11"/>
         <v>6.6</v>
       </c>
-      <c r="K40" s="27">
+      <c r="K40" s="26">
         <f t="shared" si="11"/>
         <v>6.6</v>
       </c>
-      <c r="L40" s="27">
+      <c r="L40" s="26">
         <f t="shared" si="11"/>
         <v>6.6</v>
       </c>
@@ -12457,42 +12467,42 @@
       <c r="A41" t="s">
         <v>7</v>
       </c>
-      <c r="C41" s="27">
+      <c r="C41" s="26">
         <v>0.75</v>
       </c>
-      <c r="D41" s="27">
+      <c r="D41" s="26">
         <f t="shared" si="11"/>
         <v>0.75</v>
       </c>
-      <c r="E41" s="27">
+      <c r="E41" s="26">
         <f t="shared" si="11"/>
         <v>0.75</v>
       </c>
-      <c r="F41" s="27">
+      <c r="F41" s="26">
         <f t="shared" si="11"/>
         <v>0.75</v>
       </c>
-      <c r="G41" s="27">
+      <c r="G41" s="26">
         <f t="shared" si="11"/>
         <v>0.75</v>
       </c>
-      <c r="H41" s="27">
+      <c r="H41" s="26">
         <f t="shared" si="11"/>
         <v>0.75</v>
       </c>
-      <c r="I41" s="27">
+      <c r="I41" s="26">
         <f t="shared" si="11"/>
         <v>0.75</v>
       </c>
-      <c r="J41" s="27">
+      <c r="J41" s="26">
         <f t="shared" si="11"/>
         <v>0.75</v>
       </c>
-      <c r="K41" s="27">
+      <c r="K41" s="26">
         <f t="shared" si="11"/>
         <v>0.75</v>
       </c>
-      <c r="L41" s="27">
+      <c r="L41" s="26">
         <f t="shared" si="11"/>
         <v>0.75</v>
       </c>
@@ -12784,20 +12794,20 @@
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C5" s="14" t="s">
         <v>9</v>
@@ -12830,48 +12840,48 @@
         <v>49</v>
       </c>
       <c r="M5" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="N5" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="O5" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="N5" s="14" t="s">
+      <c r="P5" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="O5" s="14" t="s">
+      <c r="Q5" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="P5" s="14" t="s">
+      <c r="R5" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="Q5" s="14" t="s">
+      <c r="S5" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="R5" s="14" t="s">
+      <c r="T5" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="S5" s="14" t="s">
+      <c r="U5" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="T5" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="U5" s="14" t="s">
-        <v>95</v>
-      </c>
       <c r="V5" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="W5" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="X5" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B6" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C6" s="2">
         <v>12.4</v>
@@ -12948,385 +12958,385 @@
         <f t="shared" si="0"/>
         <v>12.4</v>
       </c>
-      <c r="V6" s="44">
+      <c r="V6" s="31">
         <f>AVERAGE(C6:L6)</f>
         <v>12.400000000000002</v>
       </c>
-      <c r="W6" s="44">
+      <c r="W6" s="31">
         <f>AVERAGE(C6:U6)</f>
         <v>12.400000000000004</v>
       </c>
       <c r="X6" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B7" t="s">
-        <v>86</v>
-      </c>
-      <c r="C7" s="44">
+        <v>84</v>
+      </c>
+      <c r="C7" s="31">
         <v>10.541308000000001</v>
       </c>
-      <c r="D7" s="44">
+      <c r="D7" s="31">
         <v>11.023149</v>
       </c>
-      <c r="E7" s="44">
+      <c r="E7" s="31">
         <v>5.870736</v>
       </c>
-      <c r="F7" s="44">
+      <c r="F7" s="31">
         <v>10.455249</v>
       </c>
-      <c r="G7" s="44">
+      <c r="G7" s="31">
         <v>9.4432220000000004</v>
       </c>
-      <c r="H7" s="44">
+      <c r="H7" s="31">
         <v>17.117932</v>
       </c>
-      <c r="I7" s="44">
+      <c r="I7" s="31">
         <v>12.627808</v>
       </c>
-      <c r="J7" s="44">
+      <c r="J7" s="31">
         <v>12.567529</v>
       </c>
-      <c r="K7" s="44">
+      <c r="K7" s="31">
         <v>16.3156</v>
       </c>
-      <c r="L7" s="44">
+      <c r="L7" s="31">
         <v>14.306982</v>
       </c>
-      <c r="M7" s="44">
+      <c r="M7" s="31">
         <v>12.326231999999999</v>
       </c>
-      <c r="N7" s="44">
+      <c r="N7" s="31">
         <v>20.207163000000001</v>
       </c>
-      <c r="O7" s="44">
+      <c r="O7" s="31">
         <v>8.4420540000000006</v>
       </c>
-      <c r="P7" s="44">
+      <c r="P7" s="31">
         <v>8.9732859999999999</v>
       </c>
-      <c r="Q7" s="44">
+      <c r="Q7" s="31">
         <v>14.100669999999999</v>
       </c>
-      <c r="R7" s="44">
+      <c r="R7" s="31">
         <v>13.433123999999999</v>
       </c>
-      <c r="S7" s="44">
+      <c r="S7" s="31">
         <v>13.477814</v>
       </c>
-      <c r="T7" s="44">
+      <c r="T7" s="31">
         <v>16.476396999999999</v>
       </c>
-      <c r="U7" s="44">
+      <c r="U7" s="31">
         <v>8.6142029999999998</v>
       </c>
-      <c r="V7" s="44">
+      <c r="V7" s="31">
         <f t="shared" ref="V7:V13" si="1">AVERAGE(C7:L7)</f>
         <v>12.026951499999999</v>
       </c>
-      <c r="W7" s="44">
+      <c r="W7" s="31">
         <f t="shared" ref="W7:W13" si="2">AVERAGE(C7:U7)</f>
         <v>12.437918842105264</v>
       </c>
       <c r="X7" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B8" t="s">
-        <v>101</v>
-      </c>
-      <c r="C8" s="44">
+        <v>99</v>
+      </c>
+      <c r="C8" s="31">
         <f>INDEX($C$7:$U$7, _xlfn.RANK.EQ(C19, $C19:$U19) + COUNTIF($C19:C19, C19) - 1)</f>
         <v>12.627808</v>
       </c>
-      <c r="D8" s="44">
+      <c r="D8" s="31">
         <f>INDEX($C$7:$U$7, _xlfn.RANK.EQ(D19, $C19:$U19) + COUNTIF($C19:D19, D19) - 1)</f>
         <v>12.326231999999999</v>
       </c>
-      <c r="E8" s="44">
+      <c r="E8" s="31">
         <f>INDEX($C$7:$U$7, _xlfn.RANK.EQ(E19, $C19:$U19) + COUNTIF($C19:E19, E19) - 1)</f>
         <v>10.455249</v>
       </c>
-      <c r="F8" s="44">
+      <c r="F8" s="31">
         <f>INDEX($C$7:$U$7, _xlfn.RANK.EQ(F19, $C19:$U19) + COUNTIF($C19:F19, F19) - 1)</f>
         <v>5.870736</v>
       </c>
-      <c r="G8" s="44">
+      <c r="G8" s="31">
         <f>INDEX($C$7:$U$7, _xlfn.RANK.EQ(G19, $C19:$U19) + COUNTIF($C19:G19, G19) - 1)</f>
         <v>14.100669999999999</v>
       </c>
-      <c r="H8" s="44">
+      <c r="H8" s="31">
         <f>INDEX($C$7:$U$7, _xlfn.RANK.EQ(H19, $C19:$U19) + COUNTIF($C19:H19, H19) - 1)</f>
         <v>10.541308000000001</v>
       </c>
-      <c r="I8" s="44">
+      <c r="I8" s="31">
         <f>INDEX($C$7:$U$7, _xlfn.RANK.EQ(I19, $C19:$U19) + COUNTIF($C19:I19, I19) - 1)</f>
         <v>17.117932</v>
       </c>
-      <c r="J8" s="44">
+      <c r="J8" s="31">
         <f>INDEX($C$7:$U$7, _xlfn.RANK.EQ(J19, $C19:$U19) + COUNTIF($C19:J19, J19) - 1)</f>
         <v>9.4432220000000004</v>
       </c>
-      <c r="K8" s="44">
+      <c r="K8" s="31">
         <f>INDEX($C$7:$U$7, _xlfn.RANK.EQ(K19, $C19:$U19) + COUNTIF($C19:K19, K19) - 1)</f>
         <v>20.207163000000001</v>
       </c>
-      <c r="L8" s="44">
+      <c r="L8" s="31">
         <f>INDEX($C$7:$U$7, _xlfn.RANK.EQ(L19, $C19:$U19) + COUNTIF($C19:L19, L19) - 1)</f>
         <v>12.567529</v>
       </c>
-      <c r="M8" s="44">
+      <c r="M8" s="31">
         <f>INDEX($C$7:$U$7, _xlfn.RANK.EQ(M19, $C19:$U19) + COUNTIF($C19:M19, M19) - 1)</f>
         <v>14.306982</v>
       </c>
-      <c r="N8" s="44">
+      <c r="N8" s="31">
         <f>INDEX($C$7:$U$7, _xlfn.RANK.EQ(N19, $C19:$U19) + COUNTIF($C19:N19, N19) - 1)</f>
         <v>11.023149</v>
       </c>
-      <c r="O8" s="44">
+      <c r="O8" s="31">
         <f>INDEX($C$7:$U$7, _xlfn.RANK.EQ(O19, $C19:$U19) + COUNTIF($C19:O19, O19) - 1)</f>
         <v>8.4420540000000006</v>
       </c>
-      <c r="P8" s="44">
+      <c r="P8" s="31">
         <f>INDEX($C$7:$U$7, _xlfn.RANK.EQ(P19, $C19:$U19) + COUNTIF($C19:P19, P19) - 1)</f>
         <v>8.9732859999999999</v>
       </c>
-      <c r="Q8" s="44">
+      <c r="Q8" s="31">
         <f>INDEX($C$7:$U$7, _xlfn.RANK.EQ(Q19, $C19:$U19) + COUNTIF($C19:Q19, Q19) - 1)</f>
         <v>16.476396999999999</v>
       </c>
-      <c r="R8" s="44">
+      <c r="R8" s="31">
         <f>INDEX($C$7:$U$7, _xlfn.RANK.EQ(R19, $C19:$U19) + COUNTIF($C19:R19, R19) - 1)</f>
         <v>16.3156</v>
       </c>
-      <c r="S8" s="44">
+      <c r="S8" s="31">
         <f>INDEX($C$7:$U$7, _xlfn.RANK.EQ(S19, $C19:$U19) + COUNTIF($C19:S19, S19) - 1)</f>
         <v>13.477814</v>
       </c>
-      <c r="T8" s="44">
+      <c r="T8" s="31">
         <f>INDEX($C$7:$U$7, _xlfn.RANK.EQ(T19, $C19:$U19) + COUNTIF($C19:T19, T19) - 1)</f>
         <v>13.433123999999999</v>
       </c>
-      <c r="U8" s="44">
+      <c r="U8" s="31">
         <f>INDEX($C$7:$U$7, _xlfn.RANK.EQ(U19, $C19:$U19) + COUNTIF($C19:U19, U19) - 1)</f>
         <v>8.6142029999999998</v>
       </c>
-      <c r="V8" s="44">
+      <c r="V8" s="31">
         <f t="shared" si="1"/>
         <v>12.525784900000001</v>
       </c>
-      <c r="W8" s="44">
+      <c r="W8" s="31">
         <f t="shared" si="2"/>
         <v>12.437918842105264</v>
       </c>
       <c r="X8" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B9" t="s">
-        <v>102</v>
-      </c>
-      <c r="C9" s="44">
+        <v>100</v>
+      </c>
+      <c r="C9" s="31">
         <f>INDEX($C$7:$U$7, _xlfn.RANK.EQ(C20, $C20:$U20) + COUNTIF($C20:C20, C20) - 1)</f>
         <v>17.117932</v>
       </c>
-      <c r="D9" s="44">
+      <c r="D9" s="31">
         <f>INDEX($C$7:$U$7, _xlfn.RANK.EQ(D20, $C20:$U20) + COUNTIF($C20:D20, D20) - 1)</f>
         <v>10.541308000000001</v>
       </c>
-      <c r="E9" s="44">
+      <c r="E9" s="31">
         <f>INDEX($C$7:$U$7, _xlfn.RANK.EQ(E20, $C20:$U20) + COUNTIF($C20:E20, E20) - 1)</f>
         <v>14.100669999999999</v>
       </c>
-      <c r="F9" s="44">
+      <c r="F9" s="31">
         <f>INDEX($C$7:$U$7, _xlfn.RANK.EQ(F20, $C20:$U20) + COUNTIF($C20:F20, F20) - 1)</f>
         <v>14.306982</v>
       </c>
-      <c r="G9" s="44">
+      <c r="G9" s="31">
         <f>INDEX($C$7:$U$7, _xlfn.RANK.EQ(G20, $C20:$U20) + COUNTIF($C20:G20, G20) - 1)</f>
         <v>8.6142029999999998</v>
       </c>
-      <c r="H9" s="44">
+      <c r="H9" s="31">
         <f>INDEX($C$7:$U$7, _xlfn.RANK.EQ(H20, $C20:$U20) + COUNTIF($C20:H20, H20) - 1)</f>
         <v>12.326231999999999</v>
       </c>
-      <c r="I9" s="44">
+      <c r="I9" s="31">
         <f>INDEX($C$7:$U$7, _xlfn.RANK.EQ(I20, $C20:$U20) + COUNTIF($C20:I20, I20) - 1)</f>
         <v>10.455249</v>
       </c>
-      <c r="J9" s="44">
+      <c r="J9" s="31">
         <f>INDEX($C$7:$U$7, _xlfn.RANK.EQ(J20, $C20:$U20) + COUNTIF($C20:J20, J20) - 1)</f>
         <v>5.870736</v>
       </c>
-      <c r="K9" s="44">
+      <c r="K9" s="31">
         <f>INDEX($C$7:$U$7, _xlfn.RANK.EQ(K20, $C20:$U20) + COUNTIF($C20:K20, K20) - 1)</f>
         <v>13.433123999999999</v>
       </c>
-      <c r="L9" s="44">
+      <c r="L9" s="31">
         <f>INDEX($C$7:$U$7, _xlfn.RANK.EQ(L20, $C20:$U20) + COUNTIF($C20:L20, L20) - 1)</f>
         <v>11.023149</v>
       </c>
-      <c r="M9" s="44">
+      <c r="M9" s="31">
         <f>INDEX($C$7:$U$7, _xlfn.RANK.EQ(M20, $C20:$U20) + COUNTIF($C20:M20, M20) - 1)</f>
         <v>8.4420540000000006</v>
       </c>
-      <c r="N9" s="44">
+      <c r="N9" s="31">
         <f>INDEX($C$7:$U$7, _xlfn.RANK.EQ(N20, $C20:$U20) + COUNTIF($C20:N20, N20) - 1)</f>
         <v>16.476396999999999</v>
       </c>
-      <c r="O9" s="44">
+      <c r="O9" s="31">
         <f>INDEX($C$7:$U$7, _xlfn.RANK.EQ(O20, $C20:$U20) + COUNTIF($C20:O20, O20) - 1)</f>
         <v>20.207163000000001</v>
       </c>
-      <c r="P9" s="44">
+      <c r="P9" s="31">
         <f>INDEX($C$7:$U$7, _xlfn.RANK.EQ(P20, $C20:$U20) + COUNTIF($C20:P20, P20) - 1)</f>
         <v>12.567529</v>
       </c>
-      <c r="Q9" s="44">
+      <c r="Q9" s="31">
         <f>INDEX($C$7:$U$7, _xlfn.RANK.EQ(Q20, $C20:$U20) + COUNTIF($C20:Q20, Q20) - 1)</f>
         <v>8.9732859999999999</v>
       </c>
-      <c r="R9" s="44">
+      <c r="R9" s="31">
         <f>INDEX($C$7:$U$7, _xlfn.RANK.EQ(R20, $C20:$U20) + COUNTIF($C20:R20, R20) - 1)</f>
         <v>12.627808</v>
       </c>
-      <c r="S9" s="44">
+      <c r="S9" s="31">
         <f>INDEX($C$7:$U$7, _xlfn.RANK.EQ(S20, $C20:$U20) + COUNTIF($C20:S20, S20) - 1)</f>
         <v>13.477814</v>
       </c>
-      <c r="T9" s="44">
+      <c r="T9" s="31">
         <f>INDEX($C$7:$U$7, _xlfn.RANK.EQ(T20, $C20:$U20) + COUNTIF($C20:T20, T20) - 1)</f>
         <v>9.4432220000000004</v>
       </c>
-      <c r="U9" s="44">
+      <c r="U9" s="31">
         <f>INDEX($C$7:$U$7, _xlfn.RANK.EQ(U20, $C20:$U20) + COUNTIF($C20:U20, U20) - 1)</f>
         <v>16.3156</v>
       </c>
-      <c r="V9" s="44">
+      <c r="V9" s="31">
         <f t="shared" si="1"/>
         <v>11.7789585</v>
       </c>
-      <c r="W9" s="44">
+      <c r="W9" s="31">
         <f t="shared" si="2"/>
         <v>12.437918842105262</v>
       </c>
       <c r="X9" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B10" t="s">
-        <v>103</v>
-      </c>
-      <c r="C10" s="44">
+        <v>101</v>
+      </c>
+      <c r="C10" s="31">
         <f>INDEX($C$7:$U$7, _xlfn.RANK.EQ(C21, $C21:$U21) + COUNTIF($C21:C21, C21) - 1)</f>
         <v>20.207163000000001</v>
       </c>
-      <c r="D10" s="44">
+      <c r="D10" s="31">
         <f>INDEX($C$7:$U$7, _xlfn.RANK.EQ(D21, $C21:$U21) + COUNTIF($C21:D21, D21) - 1)</f>
         <v>17.117932</v>
       </c>
-      <c r="E10" s="44">
+      <c r="E10" s="31">
         <f>INDEX($C$7:$U$7, _xlfn.RANK.EQ(E21, $C21:$U21) + COUNTIF($C21:E21, E21) - 1)</f>
         <v>16.476396999999999</v>
       </c>
-      <c r="F10" s="44">
+      <c r="F10" s="31">
         <f>INDEX($C$7:$U$7, _xlfn.RANK.EQ(F21, $C21:$U21) + COUNTIF($C21:F21, F21) - 1)</f>
         <v>12.326231999999999</v>
       </c>
-      <c r="G10" s="44">
+      <c r="G10" s="31">
         <f>INDEX($C$7:$U$7, _xlfn.RANK.EQ(G21, $C21:$U21) + COUNTIF($C21:G21, G21) - 1)</f>
         <v>12.627808</v>
       </c>
-      <c r="H10" s="44">
+      <c r="H10" s="31">
         <f>INDEX($C$7:$U$7, _xlfn.RANK.EQ(H21, $C21:$U21) + COUNTIF($C21:H21, H21) - 1)</f>
         <v>13.433123999999999</v>
       </c>
-      <c r="I10" s="44">
+      <c r="I10" s="31">
         <f>INDEX($C$7:$U$7, _xlfn.RANK.EQ(I21, $C21:$U21) + COUNTIF($C21:I21, I21) - 1)</f>
         <v>10.541308000000001</v>
       </c>
-      <c r="J10" s="44">
+      <c r="J10" s="31">
         <f>INDEX($C$7:$U$7, _xlfn.RANK.EQ(J21, $C21:$U21) + COUNTIF($C21:J21, J21) - 1)</f>
         <v>16.3156</v>
       </c>
-      <c r="K10" s="44">
+      <c r="K10" s="31">
         <f>INDEX($C$7:$U$7, _xlfn.RANK.EQ(K21, $C21:$U21) + COUNTIF($C21:K21, K21) - 1)</f>
         <v>9.4432220000000004</v>
       </c>
-      <c r="L10" s="44">
+      <c r="L10" s="31">
         <f>INDEX($C$7:$U$7, _xlfn.RANK.EQ(L21, $C21:$U21) + COUNTIF($C21:L21, L21) - 1)</f>
         <v>14.306982</v>
       </c>
-      <c r="M10" s="44">
+      <c r="M10" s="31">
         <f>INDEX($C$7:$U$7, _xlfn.RANK.EQ(M21, $C21:$U21) + COUNTIF($C21:M21, M21) - 1)</f>
         <v>8.6142029999999998</v>
       </c>
-      <c r="N10" s="44">
+      <c r="N10" s="31">
         <f>INDEX($C$7:$U$7, _xlfn.RANK.EQ(N21, $C21:$U21) + COUNTIF($C21:N21, N21) - 1)</f>
         <v>10.455249</v>
       </c>
-      <c r="O10" s="44">
+      <c r="O10" s="31">
         <f>INDEX($C$7:$U$7, _xlfn.RANK.EQ(O21, $C21:$U21) + COUNTIF($C21:O21, O21) - 1)</f>
         <v>8.4420540000000006</v>
       </c>
-      <c r="P10" s="44">
+      <c r="P10" s="31">
         <f>INDEX($C$7:$U$7, _xlfn.RANK.EQ(P21, $C21:$U21) + COUNTIF($C21:P21, P21) - 1)</f>
         <v>8.9732859999999999</v>
       </c>
-      <c r="Q10" s="44">
+      <c r="Q10" s="31">
         <f>INDEX($C$7:$U$7, _xlfn.RANK.EQ(Q21, $C21:$U21) + COUNTIF($C21:Q21, Q21) - 1)</f>
         <v>14.100669999999999</v>
       </c>
-      <c r="R10" s="44">
+      <c r="R10" s="31">
         <f>INDEX($C$7:$U$7, _xlfn.RANK.EQ(R21, $C21:$U21) + COUNTIF($C21:R21, R21) - 1)</f>
         <v>13.477814</v>
       </c>
-      <c r="S10" s="44">
+      <c r="S10" s="31">
         <f>INDEX($C$7:$U$7, _xlfn.RANK.EQ(S21, $C21:$U21) + COUNTIF($C21:S21, S21) - 1)</f>
         <v>5.870736</v>
       </c>
-      <c r="T10" s="44">
+      <c r="T10" s="31">
         <f>INDEX($C$7:$U$7, _xlfn.RANK.EQ(T21, $C21:$U21) + COUNTIF($C21:T21, T21) - 1)</f>
         <v>12.567529</v>
       </c>
-      <c r="U10" s="44">
+      <c r="U10" s="31">
         <f>INDEX($C$7:$U$7, _xlfn.RANK.EQ(U21, $C21:$U21) + COUNTIF($C21:U21, U21) - 1)</f>
         <v>11.023149</v>
       </c>
-      <c r="V10" s="44">
+      <c r="V10" s="31">
         <f t="shared" si="1"/>
         <v>14.279576800000001</v>
       </c>
-      <c r="W10" s="44">
+      <c r="W10" s="31">
         <f t="shared" si="2"/>
         <v>12.437918842105265</v>
       </c>
       <c r="X10" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B11" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C11" s="2">
         <v>11.4</v>
@@ -13403,621 +13413,621 @@
         <f t="shared" si="3"/>
         <v>11.4</v>
       </c>
-      <c r="V11" s="44">
+      <c r="V11" s="31">
         <f t="shared" si="1"/>
         <v>11.400000000000002</v>
       </c>
-      <c r="W11" s="44">
+      <c r="W11" s="31">
         <f t="shared" si="2"/>
         <v>11.400000000000004</v>
       </c>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B12" t="s">
-        <v>108</v>
-      </c>
-      <c r="C12" s="44">
+        <v>106</v>
+      </c>
+      <c r="C12" s="31">
         <v>8.0656773127944597</v>
       </c>
-      <c r="D12" s="44">
+      <c r="D12" s="31">
         <v>12.179497010248401</v>
       </c>
-      <c r="E12" s="44">
+      <c r="E12" s="31">
         <v>10.4021452093777</v>
       </c>
-      <c r="F12" s="44">
+      <c r="F12" s="31">
         <v>13.518813794409299</v>
       </c>
-      <c r="G12" s="44">
+      <c r="G12" s="31">
         <v>16.316885566837801</v>
       </c>
-      <c r="H12" s="44">
+      <c r="H12" s="31">
         <v>8.2963173615850092</v>
       </c>
-      <c r="I12" s="44">
+      <c r="I12" s="31">
         <v>8.2334084440403892</v>
       </c>
-      <c r="J12" s="44">
+      <c r="J12" s="31">
         <v>8.0507265516528701</v>
       </c>
-      <c r="K12" s="44">
+      <c r="K12" s="31">
         <v>10.939025533005399</v>
       </c>
-      <c r="L12" s="44">
+      <c r="L12" s="31">
         <v>17.117619193537298</v>
       </c>
-      <c r="M12" s="44">
+      <c r="M12" s="31">
         <v>15.180122066368499</v>
       </c>
-      <c r="N12" s="44">
+      <c r="N12" s="31">
         <v>18.434952033152101</v>
       </c>
-      <c r="O12" s="44">
+      <c r="O12" s="31">
         <v>12.0058419359474</v>
       </c>
-      <c r="P12" s="44">
+      <c r="P12" s="31">
         <v>6.7697458167134199</v>
       </c>
-      <c r="Q12" s="44">
+      <c r="Q12" s="31">
         <v>14.549174163850401</v>
       </c>
-      <c r="R12" s="44">
+      <c r="R12" s="31">
         <v>7.0958145122825593</v>
       </c>
-      <c r="S12" s="44">
+      <c r="S12" s="31">
         <v>14.9052393166876</v>
       </c>
-      <c r="T12" s="44">
+      <c r="T12" s="31">
         <v>15.428213164007099</v>
       </c>
-      <c r="U12" s="44">
+      <c r="U12" s="31">
         <v>17.679933099266101</v>
       </c>
-      <c r="V12" s="44">
+      <c r="V12" s="31">
         <f t="shared" si="1"/>
         <v>11.312011597748862</v>
       </c>
-      <c r="W12" s="44">
+      <c r="W12" s="31">
         <f t="shared" si="2"/>
         <v>12.377323793987571</v>
       </c>
       <c r="X12" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B13" t="s">
-        <v>108</v>
-      </c>
-      <c r="C13" s="44">
+        <v>106</v>
+      </c>
+      <c r="C13" s="31">
         <v>13.6721827614197</v>
       </c>
-      <c r="D13" s="44">
+      <c r="D13" s="31">
         <v>12.666445529103701</v>
       </c>
-      <c r="E13" s="44">
+      <c r="E13" s="31">
         <v>8.2123208856145009</v>
       </c>
-      <c r="F13" s="44">
+      <c r="F13" s="31">
         <v>7.2985106981092596</v>
       </c>
-      <c r="G13" s="44">
+      <c r="G13" s="31">
         <v>8.9240344766710908</v>
       </c>
-      <c r="H13" s="44">
+      <c r="H13" s="31">
         <v>12.2239805462057</v>
       </c>
-      <c r="I13" s="44">
+      <c r="I13" s="31">
         <v>12.116028475951</v>
       </c>
-      <c r="J13" s="44">
+      <c r="J13" s="31">
         <v>9.3868894956851907</v>
       </c>
-      <c r="K13" s="44">
+      <c r="K13" s="31">
         <v>5.7100895102609304</v>
       </c>
-      <c r="L13" s="44">
+      <c r="L13" s="31">
         <v>7.6367030909024995</v>
       </c>
-      <c r="M13" s="44">
+      <c r="M13" s="31">
         <v>17.908698431934599</v>
       </c>
-      <c r="N13" s="44">
+      <c r="N13" s="31">
         <v>17.3439222124933</v>
       </c>
-      <c r="O13" s="44">
+      <c r="O13" s="31">
         <v>16.712138882108398</v>
       </c>
-      <c r="P13" s="44">
+      <c r="P13" s="31">
         <v>10.8627427743835</v>
       </c>
-      <c r="Q13" s="44">
+      <c r="Q13" s="31">
         <v>18.956338967251</v>
       </c>
-      <c r="R13" s="44">
+      <c r="R13" s="31">
         <v>22.2800107884749</v>
       </c>
-      <c r="S13" s="44">
+      <c r="S13" s="31">
         <v>19.616776674012698</v>
       </c>
-      <c r="T13" s="44">
+      <c r="T13" s="31">
         <v>14.694013971958199</v>
       </c>
-      <c r="U13" s="44">
+      <c r="U13" s="31">
         <v>13.8158034044588</v>
       </c>
-      <c r="V13" s="44">
+      <c r="V13" s="31">
         <f t="shared" si="1"/>
         <v>9.7847185469923588</v>
       </c>
-      <c r="W13" s="44">
+      <c r="W13" s="31">
         <f t="shared" si="2"/>
         <v>13.159875346157838</v>
       </c>
       <c r="X13" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
+        <v>104</v>
+      </c>
+      <c r="B14" t="s">
         <v>106</v>
       </c>
-      <c r="B14" t="s">
-        <v>108</v>
-      </c>
-      <c r="C14" s="44">
+      <c r="C14" s="31">
         <v>8.6387119999999999</v>
       </c>
-      <c r="D14" s="44">
+      <c r="D14" s="31">
         <v>16.724910999999999</v>
       </c>
-      <c r="E14" s="44">
+      <c r="E14" s="31">
         <v>23.729841</v>
       </c>
-      <c r="F14" s="44">
+      <c r="F14" s="31">
         <v>24.177980999999999</v>
       </c>
-      <c r="G14" s="44">
+      <c r="G14" s="31">
         <v>21.044574999999998</v>
       </c>
-      <c r="H14" s="44">
+      <c r="H14" s="31">
         <v>22.368445000000001</v>
       </c>
-      <c r="I14" s="44">
+      <c r="I14" s="31">
         <v>16.596464999999998</v>
       </c>
-      <c r="J14" s="44">
+      <c r="J14" s="31">
         <v>11.668810000000001</v>
       </c>
-      <c r="K14" s="44">
+      <c r="K14" s="31">
         <v>9.5522320000000001</v>
       </c>
-      <c r="L14" s="44">
+      <c r="L14" s="31">
         <v>8.9740110000000008</v>
       </c>
-      <c r="M14" s="44">
+      <c r="M14" s="31">
         <v>12.344601000000001</v>
       </c>
-      <c r="N14" s="44">
+      <c r="N14" s="31">
         <v>11.068530000000001</v>
       </c>
-      <c r="O14" s="44">
+      <c r="O14" s="31">
         <v>18.697527999999998</v>
       </c>
-      <c r="P14" s="44">
+      <c r="P14" s="31">
         <v>10.611249000000001</v>
       </c>
-      <c r="Q14" s="44">
+      <c r="Q14" s="31">
         <v>19.872761000000001</v>
       </c>
-      <c r="R14" s="44">
+      <c r="R14" s="31">
         <v>14.052944999999999</v>
       </c>
-      <c r="S14" s="44">
+      <c r="S14" s="31">
         <v>21.184925</v>
       </c>
-      <c r="T14" s="44">
+      <c r="T14" s="31">
         <v>16.968572999999999</v>
       </c>
-      <c r="U14" s="44">
+      <c r="U14" s="31">
         <v>16.452831</v>
       </c>
-      <c r="V14" s="44">
+      <c r="V14" s="31">
         <f t="shared" ref="V14" si="4">AVERAGE(C14:L14)</f>
         <v>16.347598299999998</v>
       </c>
-      <c r="W14" s="44">
+      <c r="W14" s="31">
         <f t="shared" ref="W14" si="5">AVERAGE(C14:U14)</f>
         <v>16.038417157894738</v>
       </c>
       <c r="X14" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B15" t="s">
-        <v>101</v>
-      </c>
-      <c r="C15" s="44">
+        <v>99</v>
+      </c>
+      <c r="C15" s="31">
         <f>INDEX($C$14:$U$14, _xlfn.RANK.EQ(C19, $C19:$U19) + COUNTIF($C19:C19, C19) - 1)</f>
         <v>16.596464999999998</v>
       </c>
-      <c r="D15" s="44">
+      <c r="D15" s="31">
         <f>INDEX($C$14:$U$14, _xlfn.RANK.EQ(D19, $C19:$U19) + COUNTIF($C19:D19, D19) - 1)</f>
         <v>12.344601000000001</v>
       </c>
-      <c r="E15" s="44">
+      <c r="E15" s="31">
         <f>INDEX($C$14:$U$14, _xlfn.RANK.EQ(E19, $C19:$U19) + COUNTIF($C19:E19, E19) - 1)</f>
         <v>24.177980999999999</v>
       </c>
-      <c r="F15" s="44">
+      <c r="F15" s="31">
         <f>INDEX($C$14:$U$14, _xlfn.RANK.EQ(F19, $C19:$U19) + COUNTIF($C19:F19, F19) - 1)</f>
         <v>23.729841</v>
       </c>
-      <c r="G15" s="44">
+      <c r="G15" s="31">
         <f>INDEX($C$14:$U$14, _xlfn.RANK.EQ(G19, $C19:$U19) + COUNTIF($C19:G19, G19) - 1)</f>
         <v>19.872761000000001</v>
       </c>
-      <c r="H15" s="44">
+      <c r="H15" s="31">
         <f>INDEX($C$14:$U$14, _xlfn.RANK.EQ(H19, $C19:$U19) + COUNTIF($C19:H19, H19) - 1)</f>
         <v>8.6387119999999999</v>
       </c>
-      <c r="I15" s="44">
+      <c r="I15" s="31">
         <f>INDEX($C$14:$U$14, _xlfn.RANK.EQ(I19, $C19:$U19) + COUNTIF($C19:I19, I19) - 1)</f>
         <v>22.368445000000001</v>
       </c>
-      <c r="J15" s="44">
+      <c r="J15" s="31">
         <f>INDEX($C$14:$U$14, _xlfn.RANK.EQ(J19, $C19:$U19) + COUNTIF($C19:J19, J19) - 1)</f>
         <v>21.044574999999998</v>
       </c>
-      <c r="K15" s="44">
+      <c r="K15" s="31">
         <f>INDEX($C$14:$U$14, _xlfn.RANK.EQ(K19, $C19:$U19) + COUNTIF($C19:K19, K19) - 1)</f>
         <v>11.068530000000001</v>
       </c>
-      <c r="L15" s="44">
+      <c r="L15" s="31">
         <f>INDEX($C$14:$U$14, _xlfn.RANK.EQ(L19, $C19:$U19) + COUNTIF($C19:L19, L19) - 1)</f>
         <v>11.668810000000001</v>
       </c>
-      <c r="M15" s="44">
+      <c r="M15" s="31">
         <f>INDEX($C$14:$U$14, _xlfn.RANK.EQ(M19, $C19:$U19) + COUNTIF($C19:M19, M19) - 1)</f>
         <v>8.9740110000000008</v>
       </c>
-      <c r="N15" s="44">
+      <c r="N15" s="31">
         <f>INDEX($C$14:$U$14, _xlfn.RANK.EQ(N19, $C19:$U19) + COUNTIF($C19:N19, N19) - 1)</f>
         <v>16.724910999999999</v>
       </c>
-      <c r="O15" s="44">
+      <c r="O15" s="31">
         <f>INDEX($C$14:$U$14, _xlfn.RANK.EQ(O19, $C19:$U19) + COUNTIF($C19:O19, O19) - 1)</f>
         <v>18.697527999999998</v>
       </c>
-      <c r="P15" s="44">
+      <c r="P15" s="31">
         <f>INDEX($C$14:$U$14, _xlfn.RANK.EQ(P19, $C19:$U19) + COUNTIF($C19:P19, P19) - 1)</f>
         <v>10.611249000000001</v>
       </c>
-      <c r="Q15" s="44">
+      <c r="Q15" s="31">
         <f>INDEX($C$14:$U$14, _xlfn.RANK.EQ(Q19, $C19:$U19) + COUNTIF($C19:Q19, Q19) - 1)</f>
         <v>16.968572999999999</v>
       </c>
-      <c r="R15" s="44">
+      <c r="R15" s="31">
         <f>INDEX($C$14:$U$14, _xlfn.RANK.EQ(R19, $C19:$U19) + COUNTIF($C19:R19, R19) - 1)</f>
         <v>9.5522320000000001</v>
       </c>
-      <c r="S15" s="44">
+      <c r="S15" s="31">
         <f>INDEX($C$14:$U$14, _xlfn.RANK.EQ(S19, $C19:$U19) + COUNTIF($C19:S19, S19) - 1)</f>
         <v>21.184925</v>
       </c>
-      <c r="T15" s="44">
+      <c r="T15" s="31">
         <f>INDEX($C$14:$U$14, _xlfn.RANK.EQ(T19, $C19:$U19) + COUNTIF($C19:T19, T19) - 1)</f>
         <v>14.052944999999999</v>
       </c>
-      <c r="U15" s="44">
+      <c r="U15" s="31">
         <f>INDEX($C$14:$U$14, _xlfn.RANK.EQ(U19, $C19:$U19) + COUNTIF($C19:U19, U19) - 1)</f>
         <v>16.452831</v>
       </c>
-      <c r="V15" s="44">
+      <c r="V15" s="31">
         <f t="shared" ref="V15:V16" si="6">AVERAGE(C15:L15)</f>
         <v>17.1510721</v>
       </c>
-      <c r="W15" s="44">
+      <c r="W15" s="31">
         <f t="shared" ref="W15:W16" si="7">AVERAGE(C15:U15)</f>
         <v>16.038417157894738</v>
       </c>
       <c r="X15" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B16" t="s">
-        <v>102</v>
-      </c>
-      <c r="C16" s="44">
+        <v>100</v>
+      </c>
+      <c r="C16" s="31">
         <f>INDEX($C$14:$U$14, _xlfn.RANK.EQ(C20, $C20:$U20) + COUNTIF($C20:C20, C20) - 1)</f>
         <v>22.368445000000001</v>
       </c>
-      <c r="D16" s="44">
+      <c r="D16" s="31">
         <f>INDEX($C$14:$U$14, _xlfn.RANK.EQ(D20, $C20:$U20) + COUNTIF($C20:D20, D20) - 1)</f>
         <v>8.6387119999999999</v>
       </c>
-      <c r="E16" s="44">
+      <c r="E16" s="31">
         <f>INDEX($C$14:$U$14, _xlfn.RANK.EQ(E20, $C20:$U20) + COUNTIF($C20:E20, E20) - 1)</f>
         <v>19.872761000000001</v>
       </c>
-      <c r="F16" s="44">
+      <c r="F16" s="31">
         <f>INDEX($C$14:$U$14, _xlfn.RANK.EQ(F20, $C20:$U20) + COUNTIF($C20:F20, F20) - 1)</f>
         <v>8.9740110000000008</v>
       </c>
-      <c r="G16" s="44">
+      <c r="G16" s="31">
         <f>INDEX($C$14:$U$14, _xlfn.RANK.EQ(G20, $C20:$U20) + COUNTIF($C20:G20, G20) - 1)</f>
         <v>16.452831</v>
       </c>
-      <c r="H16" s="44">
+      <c r="H16" s="31">
         <f>INDEX($C$14:$U$14, _xlfn.RANK.EQ(H20, $C20:$U20) + COUNTIF($C20:H20, H20) - 1)</f>
         <v>12.344601000000001</v>
       </c>
-      <c r="I16" s="44">
+      <c r="I16" s="31">
         <f>INDEX($C$14:$U$14, _xlfn.RANK.EQ(I20, $C20:$U20) + COUNTIF($C20:I20, I20) - 1)</f>
         <v>24.177980999999999</v>
       </c>
-      <c r="J16" s="44">
+      <c r="J16" s="31">
         <f>INDEX($C$14:$U$14, _xlfn.RANK.EQ(J20, $C20:$U20) + COUNTIF($C20:J20, J20) - 1)</f>
         <v>23.729841</v>
       </c>
-      <c r="K16" s="44">
+      <c r="K16" s="31">
         <f>INDEX($C$14:$U$14, _xlfn.RANK.EQ(K20, $C20:$U20) + COUNTIF($C20:K20, K20) - 1)</f>
         <v>14.052944999999999</v>
       </c>
-      <c r="L16" s="44">
+      <c r="L16" s="31">
         <f>INDEX($C$14:$U$14, _xlfn.RANK.EQ(L20, $C20:$U20) + COUNTIF($C20:L20, L20) - 1)</f>
         <v>16.724910999999999</v>
       </c>
-      <c r="M16" s="44">
+      <c r="M16" s="31">
         <f>INDEX($C$14:$U$14, _xlfn.RANK.EQ(M20, $C20:$U20) + COUNTIF($C20:M20, M20) - 1)</f>
         <v>18.697527999999998</v>
       </c>
-      <c r="N16" s="44">
+      <c r="N16" s="31">
         <f>INDEX($C$14:$U$14, _xlfn.RANK.EQ(N20, $C20:$U20) + COUNTIF($C20:N20, N20) - 1)</f>
         <v>16.968572999999999</v>
       </c>
-      <c r="O16" s="44">
+      <c r="O16" s="31">
         <f>INDEX($C$14:$U$14, _xlfn.RANK.EQ(O20, $C20:$U20) + COUNTIF($C20:O20, O20) - 1)</f>
         <v>11.068530000000001</v>
       </c>
-      <c r="P16" s="44">
+      <c r="P16" s="31">
         <f>INDEX($C$14:$U$14, _xlfn.RANK.EQ(P20, $C20:$U20) + COUNTIF($C20:P20, P20) - 1)</f>
         <v>11.668810000000001</v>
       </c>
-      <c r="Q16" s="44">
+      <c r="Q16" s="31">
         <f>INDEX($C$14:$U$14, _xlfn.RANK.EQ(Q20, $C20:$U20) + COUNTIF($C20:Q20, Q20) - 1)</f>
         <v>10.611249000000001</v>
       </c>
-      <c r="R16" s="44">
+      <c r="R16" s="31">
         <f>INDEX($C$14:$U$14, _xlfn.RANK.EQ(R20, $C20:$U20) + COUNTIF($C20:R20, R20) - 1)</f>
         <v>16.596464999999998</v>
       </c>
-      <c r="S16" s="44">
+      <c r="S16" s="31">
         <f>INDEX($C$14:$U$14, _xlfn.RANK.EQ(S20, $C20:$U20) + COUNTIF($C20:S20, S20) - 1)</f>
         <v>21.184925</v>
       </c>
-      <c r="T16" s="44">
+      <c r="T16" s="31">
         <f>INDEX($C$14:$U$14, _xlfn.RANK.EQ(T20, $C20:$U20) + COUNTIF($C20:T20, T20) - 1)</f>
         <v>21.044574999999998</v>
       </c>
-      <c r="U16" s="44">
+      <c r="U16" s="31">
         <f>INDEX($C$14:$U$14, _xlfn.RANK.EQ(U20, $C20:$U20) + COUNTIF($C20:U20, U20) - 1)</f>
         <v>9.5522320000000001</v>
       </c>
-      <c r="V16" s="44">
+      <c r="V16" s="31">
         <f t="shared" si="6"/>
         <v>16.733703900000002</v>
       </c>
-      <c r="W16" s="44">
+      <c r="W16" s="31">
         <f t="shared" si="7"/>
         <v>16.038417157894738</v>
       </c>
       <c r="X16" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>96</v>
-      </c>
-      <c r="C19" s="45">
+        <v>94</v>
+      </c>
+      <c r="C19" s="32">
         <v>0.67644387335744371</v>
       </c>
-      <c r="D19" s="45">
+      <c r="D19" s="32">
         <v>0.47418579468589028</v>
       </c>
-      <c r="E19" s="45">
+      <c r="E19" s="32">
         <v>0.79191284201733858</v>
       </c>
-      <c r="F19" s="45">
+      <c r="F19" s="32">
         <v>0.85845050624319708</v>
       </c>
-      <c r="G19" s="45">
+      <c r="G19" s="32">
         <v>0.29119580343142981</v>
       </c>
-      <c r="H19" s="45">
+      <c r="H19" s="32">
         <v>0.96698220369983379</v>
       </c>
-      <c r="I19" s="45">
+      <c r="I19" s="32">
         <v>0.71660723236774859</v>
       </c>
-      <c r="J19" s="45">
+      <c r="J19" s="32">
         <v>0.76657250740819849</v>
       </c>
-      <c r="K19" s="45">
+      <c r="K19" s="32">
         <v>0.37210589764212265</v>
       </c>
-      <c r="L19" s="45">
+      <c r="L19" s="32">
         <v>0.67238760239552131</v>
       </c>
-      <c r="M19" s="45">
+      <c r="M19" s="32">
         <v>0.54861280840425941</v>
       </c>
-      <c r="N19" s="45">
+      <c r="N19" s="32">
         <v>0.93847094237556061</v>
       </c>
-      <c r="O19" s="45">
+      <c r="O19" s="32">
         <v>0.37036993145978159</v>
       </c>
-      <c r="P19" s="45">
+      <c r="P19" s="32">
         <v>0.37012384678989274</v>
       </c>
-      <c r="Q19" s="45">
+      <c r="Q19" s="32">
         <v>5.0129257600194155E-2</v>
       </c>
-      <c r="R19" s="45">
+      <c r="R19" s="32">
         <v>0.66224607523003343</v>
       </c>
-      <c r="S19" s="45">
+      <c r="S19" s="32">
         <v>7.3598766477379618E-2</v>
       </c>
-      <c r="T19" s="45">
+      <c r="T19" s="32">
         <v>0.14075741794709939</v>
       </c>
-      <c r="U19" s="45">
+      <c r="U19" s="32">
         <v>4.0761876740060932E-2</v>
       </c>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>97</v>
-      </c>
-      <c r="C20" s="45">
+        <v>95</v>
+      </c>
+      <c r="C20" s="32">
         <v>0.71178139473095614</v>
       </c>
-      <c r="D20" s="45">
+      <c r="D20" s="32">
         <v>0.90508858194637953</v>
       </c>
-      <c r="E20" s="45">
+      <c r="E20" s="32">
         <v>0.17598711058710848</v>
       </c>
-      <c r="F20" s="45">
+      <c r="F20" s="32">
         <v>0.46040924842222275</v>
       </c>
-      <c r="G20" s="45">
+      <c r="G20" s="32">
         <v>1.1082729617274412E-3</v>
       </c>
-      <c r="H20" s="45">
+      <c r="H20" s="32">
         <v>0.4469646580924429</v>
       </c>
-      <c r="I20" s="45">
+      <c r="I20" s="32">
         <v>0.76533202050878746</v>
       </c>
-      <c r="J20" s="45">
+      <c r="J20" s="32">
         <v>0.83884971961311028</v>
       </c>
-      <c r="K20" s="45">
+      <c r="K20" s="32">
         <v>0.13861192500449215</v>
       </c>
-      <c r="L20" s="45">
+      <c r="L20" s="32">
         <v>0.86445706016894996</v>
       </c>
-      <c r="M20" s="45">
+      <c r="M20" s="32">
         <v>0.27880519114550062</v>
       </c>
-      <c r="N20" s="45">
+      <c r="N20" s="32">
         <v>4.9331580912537532E-2</v>
       </c>
-      <c r="O20" s="45">
+      <c r="O20" s="32">
         <v>0.44358552686154573</v>
       </c>
-      <c r="P20" s="45">
+      <c r="P20" s="32">
         <v>0.51627460025941363</v>
       </c>
-      <c r="Q20" s="45">
+      <c r="Q20" s="32">
         <v>0.19589373219881623</v>
       </c>
-      <c r="R20" s="45">
+      <c r="R20" s="32">
         <v>0.57711767229760702</v>
       </c>
-      <c r="S20" s="45">
+      <c r="S20" s="32">
         <v>0.11578704812173612</v>
       </c>
-      <c r="T20" s="45">
+      <c r="T20" s="32">
         <v>0.75445830147475079</v>
       </c>
-      <c r="U20" s="45">
+      <c r="U20" s="32">
         <v>0.50908150625985971</v>
       </c>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>98</v>
-      </c>
-      <c r="C21" s="45">
+        <v>96</v>
+      </c>
+      <c r="C21" s="32">
         <v>0.49942177488685924</v>
       </c>
-      <c r="D21" s="45">
+      <c r="D21" s="32">
         <v>0.73533205529292978</v>
       </c>
-      <c r="E21" s="45">
+      <c r="E21" s="32">
         <v>3.6281905650776269E-2</v>
       </c>
-      <c r="F21" s="45">
+      <c r="F21" s="32">
         <v>0.51032194818600674</v>
       </c>
-      <c r="G21" s="45">
+      <c r="G21" s="32">
         <v>0.72301799545372614</v>
       </c>
-      <c r="H21" s="45">
+      <c r="H21" s="32">
         <v>0.18140139614899009</v>
       </c>
-      <c r="I21" s="45">
+      <c r="I21" s="32">
         <v>0.96487922099534429</v>
       </c>
-      <c r="J21" s="45">
+      <c r="J21" s="32">
         <v>0.58598497382130921</v>
       </c>
-      <c r="K21" s="45">
+      <c r="K21" s="32">
         <v>0.81220936811505928</v>
       </c>
-      <c r="L21" s="45">
+      <c r="L21" s="32">
         <v>0.56799175094937815</v>
       </c>
-      <c r="M21" s="45">
+      <c r="M21" s="32">
         <v>1.6868147569877312E-3</v>
       </c>
-      <c r="N21" s="45">
+      <c r="N21" s="32">
         <v>0.81525247724513761</v>
       </c>
-      <c r="O21" s="45">
+      <c r="O21" s="32">
         <v>0.43869003462286138</v>
       </c>
-      <c r="P21" s="45">
+      <c r="P21" s="32">
         <v>0.41310932122101518</v>
       </c>
-      <c r="Q21" s="45">
+      <c r="Q21" s="32">
         <v>0.31390513036414502</v>
       </c>
-      <c r="R21" s="45">
+      <c r="R21" s="32">
         <v>8.330275026684264E-2</v>
       </c>
-      <c r="S21" s="45">
+      <c r="S21" s="32">
         <v>0.8318657658083044</v>
       </c>
-      <c r="T21" s="45">
+      <c r="T21" s="32">
         <v>0.65077408918348401</v>
       </c>
-      <c r="U21" s="45">
+      <c r="U21" s="32">
         <v>0.92682339319863516</v>
       </c>
     </row>

</xml_diff>